<commit_message>
Clearing and some minor changes
</commit_message>
<xml_diff>
--- a/Plan de Test.xlsx
+++ b/Plan de Test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b36a37f1b0a2abb6/DOCUMENTS/TP_BUSCOM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HUB\BUSCOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="11_67E74BF4C3BC18AAAB651B8F2C458D4721544C5E" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{607E46AB-B763-4054-9DFB-31D01C58D09B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90355764-5AF6-473B-BF77-9D2AEA6566F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9285" yWindow="-15480" windowWidth="19440" windowHeight="15000" tabRatio="848" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" tabRatio="848" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="One Wire" sheetId="36" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="73">
   <si>
     <t>Test ID</t>
   </si>
@@ -304,6 +304,50 @@
     <t>Microcontroleur STM32F446RETx (Master)
 DS1820 (Capteur Température One-Wire) 
 Module SigFox + PC pour visualiser sur internet</t>
+  </si>
+  <si>
+    <t>Allan PACCOT</t>
+  </si>
+  <si>
+    <t>Envoyer un petit mot doux à Thibault.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lecture d'un registre </t>
+  </si>
+  <si>
+    <t>NUCLEO F446RE
+Module LoRa SX1272
+Putty - PC</t>
+  </si>
+  <si>
+    <t>Affichage de la version sur le terminale du PC, (=0x22)</t>
+  </si>
+  <si>
+    <t>Envoie d'une trame et visualisation via SDRangel</t>
+  </si>
+  <si>
+    <t>NUCLEO F446RE
+Module LoRa SX1272
+Dongle TNT
+SDRangel - PC</t>
+  </si>
+  <si>
+    <t>Envoyer des mots doux entre deux module</t>
+  </si>
+  <si>
+    <t>Affichage de la reception sur Putty, et envoie en continu</t>
+  </si>
+  <si>
+    <t>Lire le registre version (0x42), lire la valeur sur Putty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Envoyer une trame en LoRa (868,5MHz) et observer l'activité frequentielle </t>
+  </si>
+  <si>
+    <t>Visualisation de l'envoie sur SDRangel (analyseur de spectre)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Envoie et reception entre deux module LoRa. Envoie periodique. </t>
   </si>
 </sst>
 </file>
@@ -654,7 +698,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -716,6 +760,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -739,9 +786,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2588,7 +2632,7 @@
   </sheetPr>
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D31" sqref="D29:D31"/>
     </sheetView>
   </sheetViews>
@@ -2729,7 +2773,7 @@
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="66" t="s">
+      <c r="A10" s="37" t="s">
         <v>55</v>
       </c>
       <c r="B10" s="38"/>
@@ -2903,7 +2947,7 @@
       <c r="G23" s="16"/>
       <c r="H23" s="16"/>
     </row>
-    <row r="24" spans="1:15" s="18" customFormat="1" ht="75" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:15" s="18" customFormat="1" ht="60" x14ac:dyDescent="0.35">
       <c r="A24" s="26" t="s">
         <v>4</v>
       </c>
@@ -2929,7 +2973,7 @@
       <c r="M24" s="17"/>
       <c r="N24" s="17"/>
     </row>
-    <row r="25" spans="1:15" s="18" customFormat="1" ht="60" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:15" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.35">
       <c r="A25" s="24" t="s">
         <v>7</v>
       </c>
@@ -2947,7 +2991,7 @@
       </c>
       <c r="F25" s="24"/>
     </row>
-    <row r="26" spans="1:15" s="18" customFormat="1" ht="75" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:15" s="18" customFormat="1" ht="60" x14ac:dyDescent="0.35">
       <c r="A26" s="24" t="s">
         <v>8</v>
       </c>
@@ -3048,8 +3092,8 @@
   </sheetPr>
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:F6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -3113,7 +3157,9 @@
         <v>11</v>
       </c>
       <c r="B4" s="50"/>
-      <c r="C4" s="9"/>
+      <c r="C4" s="9" t="s">
+        <v>60</v>
+      </c>
       <c r="D4" s="5"/>
       <c r="E4" s="54"/>
       <c r="F4" s="55"/>
@@ -3126,7 +3172,9 @@
         <v>12</v>
       </c>
       <c r="B5" s="50"/>
-      <c r="C5" s="9"/>
+      <c r="C5" s="9" t="s">
+        <v>60</v>
+      </c>
       <c r="D5" s="5"/>
       <c r="E5" s="54"/>
       <c r="F5" s="55"/>
@@ -3185,7 +3233,9 @@
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="37"/>
+      <c r="A10" s="58" t="s">
+        <v>61</v>
+      </c>
       <c r="B10" s="38"/>
       <c r="C10" s="38"/>
       <c r="D10" s="38"/>
@@ -3357,14 +3407,22 @@
       <c r="G23" s="16"/>
       <c r="H23" s="16"/>
     </row>
-    <row r="24" spans="1:15" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:15" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.35">
       <c r="A24" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="22"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="23"/>
+      <c r="B24" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="E24" s="23" t="s">
+        <v>64</v>
+      </c>
       <c r="F24" s="24"/>
       <c r="G24" s="16"/>
       <c r="H24" s="16"/>
@@ -3375,24 +3433,40 @@
       <c r="M24" s="17"/>
       <c r="N24" s="17"/>
     </row>
-    <row r="25" spans="1:15" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:15" s="18" customFormat="1" ht="60" x14ac:dyDescent="0.35">
       <c r="A25" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="22"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="25"/>
+      <c r="B25" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="E25" s="25" t="s">
+        <v>71</v>
+      </c>
       <c r="F25" s="24"/>
     </row>
-    <row r="26" spans="1:15" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:15" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.35">
       <c r="A26" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="25"/>
+      <c r="B26" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="E26" s="25" t="s">
+        <v>68</v>
+      </c>
       <c r="F26" s="24"/>
     </row>
   </sheetData>
@@ -3463,7 +3537,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="59" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="58" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <tableParts count="1">
     <tablePart r:id="rId3"/>
@@ -3533,7 +3607,7 @@
       <c r="E3" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="58"/>
+      <c r="F3" s="59"/>
       <c r="G3" s="3"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -3545,8 +3619,8 @@
       <c r="B4" s="50"/>
       <c r="C4" s="9"/>
       <c r="D4" s="5"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="61"/>
       <c r="G4" s="2"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -3558,8 +3632,8 @@
       <c r="B5" s="50"/>
       <c r="C5" s="9"/>
       <c r="D5" s="5"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="61"/>
       <c r="G5" s="2"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -3573,8 +3647,8 @@
         <v>14</v>
       </c>
       <c r="D6" s="5"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="60"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="61"/>
       <c r="G6" s="2"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -3584,8 +3658,8 @@
       <c r="B7" s="27"/>
       <c r="C7" s="28"/>
       <c r="D7" s="5"/>
-      <c r="E7" s="61"/>
-      <c r="F7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="63"/>
       <c r="G7" s="2"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -3615,7 +3689,7 @@
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="37"/>
+      <c r="A10" s="58"/>
       <c r="B10" s="38"/>
       <c r="C10" s="38"/>
       <c r="D10" s="38"/>
@@ -3963,7 +4037,7 @@
       <c r="E3" s="52" t="s">
         <v>47</v>
       </c>
-      <c r="F3" s="58"/>
+      <c r="F3" s="59"/>
       <c r="G3" s="3"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -3975,8 +4049,8 @@
       <c r="B4" s="50"/>
       <c r="C4" s="9"/>
       <c r="D4" s="5"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="61"/>
       <c r="G4" s="2"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -3988,8 +4062,8 @@
       <c r="B5" s="50"/>
       <c r="C5" s="9"/>
       <c r="D5" s="5"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="61"/>
       <c r="G5" s="2"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -4003,8 +4077,8 @@
         <v>14</v>
       </c>
       <c r="D6" s="5"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="62"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="63"/>
       <c r="G6" s="2"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -4045,7 +4119,7 @@
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="37"/>
+      <c r="A10" s="58"/>
       <c r="B10" s="38"/>
       <c r="C10" s="38"/>
       <c r="D10" s="38"/>
@@ -4347,18 +4421,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="45" x14ac:dyDescent="1.1499999999999999">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
     </row>
     <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.4">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="31" t="s">
@@ -4388,11 +4462,11 @@
       <c r="B7" s="29"/>
     </row>
     <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.4">
-      <c r="A8" s="63" t="s">
+      <c r="A8" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="63"/>
-      <c r="C8" s="63"/>
+      <c r="B8" s="64"/>
+      <c r="C8" s="64"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="31" t="s">
@@ -4454,11 +4528,11 @@
       <c r="C14" s="31"/>
     </row>
     <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.35">
-      <c r="A16" s="64" t="s">
+      <c r="A16" s="65" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="64"/>
-      <c r="C16" s="64"/>
+      <c r="B16" s="65"/>
+      <c r="C16" s="65"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="31" t="s">
@@ -4551,21 +4625,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010074C32511E968E749AFF05B57F8821AD1" ma:contentTypeVersion="0" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="d2c148ac39e7dbaa061c931ce8331fe6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7043723848d0f805fbc3fbd7bf262d25">
     <xsd:element name="properties">
@@ -4679,10 +4738,32 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF1816DE-C338-43F1-A97D-D8E4FB90C584}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7380EF3C-42F8-4AC5-A9A4-260667277D61}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
@@ -4697,16 +4778,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7380EF3C-42F8-4AC5-A9A4-260667277D61}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF1816DE-C338-43F1-A97D-D8E4FB90C584}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>